<commit_message>
Added general report stuff
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,6 +407,36 @@
           <t>Alle regelhenvisninger (forbedring)</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Aktivitetsnummer</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Rapporttittel</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Dato</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Oppgaveleder</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Deltakere_i_revisjon</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -448,6 +478,36 @@
         <is>
           <t xml:space="preserve">Rammeforskriften § 15 - God helse-, miljø- og sikkerhetskultur
 </t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://www.ptil.no//contentassets/f955a9317bff4749bfc21db88383a8a3/2020_102_rapport-palegg-tilsyn-neptune-gjoa-vedlikeholdsstyring.pdf</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">027153044 </t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">undervannsanleggene (aktivitet 027153044)  </t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">27.04.2020 </t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kenneth Skogen </t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mihajlovic </t>
         </is>
       </c>
     </row>
@@ -478,6 +538,12 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -506,6 +572,12 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -534,6 +606,12 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -562,6 +640,12 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -590,6 +674,12 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -618,6 +708,12 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -646,6 +742,12 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -674,6 +776,12 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -702,6 +810,12 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added a fix for the cut-off problem in the report title and the participants in the revision
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">undervannsanleggene (aktivitet 027153044)  </t>
+          <t xml:space="preserve">Tilsynet med styringen av vedlikeholdet på Gjøa, deriblant undervannsanleggene (aktivitet 027153044)  </t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mihajlovic </t>
+          <t xml:space="preserve">Thom Fosselie, Eirik Duesten, Kenneth Skogen, Hans Spilde, Damir Mihajlovic </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added predicted category for deviations and improvements points (ML)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,75 +389,80 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Kategori (avvik)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Forbedringspunkter</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Tittel på forbedringspunkt</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Forbedringens beskrivende tekst</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Alle regelhenvisninger (forbedring)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Kategori (forbedringer)</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Aktivitetsnummer</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Rapporttittel</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Dato</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Oppgaveleder</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Deltakere_i_revisjon</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Myndighet</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Tilsynslaget størrelse</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>År</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Antall funn</t>
         </is>
@@ -486,74 +491,79 @@
 </t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>['teknisksikkerhet']</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Mangelfull kompetanse </t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Personell innen logistikk på Draugen manglet tilstrekkelig kompetanse til å bruke løfteutstyr.</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t xml:space="preserve">Aktivitetsforskriften § 21 - Kompetanse
 </t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>category_prediction(test_imp.description)</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>['styring']</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>https://www.ptil.no//contentassets/7d74d197df714c3188c464d5ef8d987e/2020_509_rapport-tilsyn-okea-draugen-materialhandtering-kran-og-loft-arbeid-i-hoyden-arbeidsmiljo.pdf</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t xml:space="preserve">061093005 </t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t xml:space="preserve">Tilsynsrapport etter tilsyn innen materialhåndtering, kran og løft, arbeid i høyden og arbeidsmiljø på Draugen </t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t xml:space="preserve">8.5.2020 </t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t xml:space="preserve">Sigmund Andreassen </t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t xml:space="preserve">Torbjørn Gjerde, Anne Sissel Graue, Hilde Nilsen </t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>PTIL</t>
         </is>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>3</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -580,31 +590,35 @@
 </t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['styring']</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Mangelfulle arbeidsmiljøkartlegginger</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Arbeidsmiljøkartleggingene for Draugen var mangelfulle.</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t xml:space="preserve">Styringsforskriften § 18 - Analyse av arbeidsmiljøet
 </t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>category_prediction(test_imp.description)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>['teknisksikkerhet']</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -614,6 +628,7 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -638,7 +653,11 @@
 </t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['styring']</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -653,6 +672,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -677,7 +697,11 @@
 </t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['materialhåndtering']</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -692,6 +716,7 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -716,7 +741,11 @@
 </t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['styring']</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
@@ -731,6 +760,7 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -755,7 +785,11 @@
 </t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['styring']</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -770,6 +804,7 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added functionallity to search through many URLs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,77 +497,77 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Barrierestyring</t>
+          <t xml:space="preserve"> Mangler med kapasitet og kompetanse</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mangelfull ivaretakelse av krav til barrierer, herunder fastsettelse av ytelseskrav og oppfølging av tilhørende tilstand. </t>
+          <t>Det var ikke samsvar mellom tilgjengelige ressurser, kompetanse og planlagte oppgaver.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Styringsforskriften § 14 - Bemanning og kompetanse
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>['styring']</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bedre barrierestyring </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Det var enkelte mangler med strategier og prinsipper for barrierenes funksjon.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t xml:space="preserve">Styringsforskriften § 5 - Barrierer
 </t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>['teknisksikkerhet']</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Utforming av blackstart prosedyre </t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Den ansvarlige synes ikke i tilstrekkelig grad å ha utformet blackstart prosedyren på en entydig og brukervennlig måte slik at den oppfyller sin tiltenkte funksjon.</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 24 - Prosedyrer
-</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>https://www.ptil.no//contentassets/48703b73602c4b38968e0d518f685565/tilsynsrapport-etter-tilsyn-med-elektriske-anlegg-instrumenterte-sikkerhetssystemer-og-teknisk-sikkerhet-pa-petrojarl-knarr-fpso.pdf</t>
+          <t>https://www.ptil.no//contentassets/450c52df67044edfac277b1eea84925e/2020_79_rapport-tilsyn-equinor-oseberg-c-barrierestyring.pdf</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve">411003018 </t>
+          <t xml:space="preserve">001053053 </t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gradering </t>
+          <t xml:space="preserve">Tilsyn med styring av barrierer på Oseberg C </t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t xml:space="preserve">4.5.2020 </t>
+          <t xml:space="preserve">27.3.2020 </t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jan Sola Østensen </t>
+          <t xml:space="preserve">Odd Tjelta </t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Liv Ranveig Rundell, Trond Jan Øglend og Jan S. Østensen </t>
+          <t xml:space="preserve">Odd Tjelta, Kristi Wiger, Eivind Sande, Eivind Hovland, Gerhard Ersdal og Elisabeth Lootz </t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="S2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -584,11 +584,11 @@
         </is>
       </c>
       <c r="U2" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Installasjon</t>
+          <t>Not found</t>
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
@@ -599,7 +599,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Petrojarl Knarr</t>
+          <t>Not found</t>
         </is>
       </c>
     </row>
@@ -612,25 +612,23 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Vedlikeholdsstyring </t>
+          <t xml:space="preserve"> Mangler med varsling og oppfølging av brønnhendelsen 28.2.2019 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mangelfull oppfølging av sikkerhetskritisk utstyr for å sikre at disse holdes ved like, slik at de er i stand til å utføre sine funksjoner </t>
+          <t>Det var mangler med varsling og oppfølging av hendelse.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 45 - Vedlikehold
-Aktivitetsforskriften § 46 - Klassifisering
-Aktivitetsforskriften § 47 - Vedlikeholdsprogram
+          <t xml:space="preserve">Styringsforskriften § 30 - Informasjon om oppfølging av fare- og ulykkessituasjoner
 </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['teknisksikkerhet']</t>
+          <t>['vedlikehold']</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -638,17 +636,18 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Synliggjøring av beslutningsgrunnlag </t>
+          <t xml:space="preserve"> Mangler ved oppfølging av operasjonelle og organisatoriske barriereelementer</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Den ansvarlige kunne ikke dokumentere at problemstillinger som angår helse, miljø og sikkerhet, var allsidig og tilstrekkelig belyst før beslutninger treffes.  </t>
+          <t>Det var mangler ved ytelseskrav, verifikasjon av ytelse og overvåking av operasjonelle og organisatoriske barriereelementer, samt gjennomføring av treninger.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Styringsforskriften § 11 - Beslutningsgrunnlag og beslutningskriterier
+          <t xml:space="preserve">Styringsforskriften § 5 - Barrierer
+Aktivitetsforskriften § 23 - Trening og øvelser
 </t>
         </is>
       </c>
@@ -672,334 +671,6 @@
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Nødkraftsystemer </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Manglende dokumentasjon på at nødstrømsanlegg (UPS anlegg) har tilstrekkelig selektivitet mellom vern ved feil i anlegget. Det kunne heller ikke dokumenteres at det var utført vurderinger vedrørende behovet for kontinuerlig drift av forbrukere forsynt fra nødkraftsystemet. </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Innretningsforskriften § 38 - Nødkraft og nødbelysning
-</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Kartlegging av potensielle tennkilder </t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mangler ved systematisk kartlegging av potensielle tennkilder.  </t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Innretningsforskriften § 10a - Tennkildekontroll
-</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Nødbelysning </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Det var ikke sikret at nødlysanlegget gir nødvendig belysning i kritiske områder ved utfall av øvrig belysning. </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Styringsforskriften § 5 - Barrierer
-Innretningsforskriften § 38 - Nødkraft og nødbelysning
-</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Rutiner for lagerhold </t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Selskapet kunne ikke vise til rutiner for ivaretakelse av teknisk tilstand til utstyr på lager. </t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 16 - Installering og ferdigstilling
-</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Konsekvens av verste brann  </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Det kunne ikke dokumenteres at en eventuell verste prosessbrann (worst credible process fire) ikke eskalerer ut av brannområdet.  </t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Innretningsforskriften § 30 - Brannskiller
-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Risikovurdering av helsefare ved elektromagnetiske felt   </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Manglende kartlegging og dokumentasjon av i hvilken utstrekning arbeidstakerne utsettes for elektromagnetiske felt utover fastsatte grenseverdier.  </t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 37 - Stråling
-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Arbeid i og drift av elektriske anlegg </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mangler ved iverksettelse og oppfølging av robustgjøringstiltak for å unngå fare- og ulykkessituasjoner knyttet til arbeid i og drift av elektriske anlegg. </t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 21 - Kompetanse
-Aktivitetsforskriften § 91 - Arbeid i og drift av elektriske anlegg
-</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Manglende kompetanse for kommunikasjonsansvarlig   </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Den ansvarlige kunne ikke dokumentere at kommunikasjonsansvarlig har den nødvendige kompetansen for å kunne utføre aktivitetene i henhold til helse-, miljø- og sikkerhetslovgivningen. </t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aktivitetsforskriften § 21 - Kompetanse
-</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>['teknisksikkerhet']</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>